<commit_message>
Mods for Hl7 UK site
</commit_message>
<xml_diff>
--- a/docs/CareConnect-Observation-1.xlsx
+++ b/docs/CareConnect-Observation-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4203" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4203" uniqueCount="561">
   <si>
     <t>Path</t>
   </si>
@@ -1699,10 +1699,6 @@
   </si>
   <si>
     <t>Observation.component.code.coding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value:code}
-</t>
   </si>
   <si>
     <t>Observation.component.code.coding.id</t>
@@ -13534,7 +13530,7 @@
         <v>45</v>
       </c>
       <c r="AA99" t="s" s="2">
-        <v>541</v>
+        <v>235</v>
       </c>
       <c r="AB99" s="2"/>
       <c r="AC99" t="s" s="2">
@@ -13700,7 +13696,7 @@
     </row>
     <row r="101" hidden="true">
       <c r="A101" t="s" s="2">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" t="s" s="2">
@@ -13815,7 +13811,7 @@
     </row>
     <row r="102" hidden="true">
       <c r="A102" t="s" s="2">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" t="s" s="2">
@@ -13930,7 +13926,7 @@
     </row>
     <row r="103" hidden="true">
       <c r="A103" t="s" s="2">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B103" t="s" s="2">
         <v>246</v>
@@ -14047,7 +14043,7 @@
     </row>
     <row r="104" hidden="true">
       <c r="A104" t="s" s="2">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B104" s="2"/>
       <c r="C104" t="s" s="2">
@@ -14166,7 +14162,7 @@
     </row>
     <row r="105" hidden="true">
       <c r="A105" t="s" s="2">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B105" s="2"/>
       <c r="C105" t="s" s="2">
@@ -14283,7 +14279,7 @@
     </row>
     <row r="106" hidden="true">
       <c r="A106" t="s" s="2">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B106" s="2"/>
       <c r="C106" t="s" s="2">
@@ -14400,7 +14396,7 @@
     </row>
     <row r="107" hidden="true">
       <c r="A107" t="s" s="2">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B107" s="2"/>
       <c r="C107" t="s" s="2">
@@ -14517,7 +14513,7 @@
     </row>
     <row r="108" hidden="true">
       <c r="A108" t="s" s="2">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B108" s="2"/>
       <c r="C108" t="s" s="2">
@@ -14636,7 +14632,7 @@
     </row>
     <row r="109" hidden="true">
       <c r="A109" t="s" s="2">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B109" s="2"/>
       <c r="C109" t="s" s="2">
@@ -14755,7 +14751,7 @@
     </row>
     <row r="110" hidden="true">
       <c r="A110" t="s" s="2">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B110" s="2"/>
       <c r="C110" t="s" s="2">
@@ -14778,16 +14774,16 @@
         <v>57</v>
       </c>
       <c r="J110" t="s" s="2">
+        <v>550</v>
+      </c>
+      <c r="K110" t="s" s="2">
         <v>551</v>
-      </c>
-      <c r="K110" t="s" s="2">
-        <v>552</v>
       </c>
       <c r="L110" t="s" s="2">
         <v>349</v>
       </c>
       <c r="M110" t="s" s="2">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="N110" t="s" s="2">
         <v>351</v>
@@ -14839,7 +14835,7 @@
         <v>45</v>
       </c>
       <c r="AE110" t="s" s="2">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="AF110" t="s" s="2">
         <v>43</v>
@@ -14857,7 +14853,7 @@
         <v>45</v>
       </c>
       <c r="AK110" t="s" s="2">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="AL110" t="s" s="2">
         <v>355</v>
@@ -14874,7 +14870,7 @@
     </row>
     <row r="111" hidden="true">
       <c r="A111" t="s" s="2">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B111" s="2"/>
       <c r="C111" t="s" s="2">
@@ -14900,13 +14896,13 @@
         <v>142</v>
       </c>
       <c r="K111" t="s" s="2">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="L111" t="s" s="2">
         <v>360</v>
       </c>
       <c r="M111" t="s" s="2">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="N111" t="s" s="2">
         <v>362</v>
@@ -14958,7 +14954,7 @@
         <v>45</v>
       </c>
       <c r="AE111" t="s" s="2">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="AF111" t="s" s="2">
         <v>43</v>
@@ -14993,7 +14989,7 @@
     </row>
     <row r="112" hidden="true">
       <c r="A112" t="s" s="2">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B112" s="2"/>
       <c r="C112" t="s" s="2">
@@ -15025,7 +15021,7 @@
         <v>370</v>
       </c>
       <c r="M112" t="s" s="2">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="N112" t="s" s="2">
         <v>371</v>
@@ -15077,7 +15073,7 @@
         <v>45</v>
       </c>
       <c r="AE112" t="s" s="2">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="AF112" t="s" s="2">
         <v>43</v>
@@ -15112,7 +15108,7 @@
     </row>
     <row r="113" hidden="true">
       <c r="A113" t="s" s="2">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" t="s" s="2">
@@ -15138,7 +15134,7 @@
         <v>45</v>
       </c>
       <c r="K113" t="s" s="2">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="L113" t="s" s="2">
         <v>451</v>
@@ -15196,7 +15192,7 @@
         <v>45</v>
       </c>
       <c r="AE113" t="s" s="2">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="AF113" t="s" s="2">
         <v>43</v>

</xml_diff>